<commit_message>
comparacion fuzzy done tomo
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Fuzzy/DataLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Fuzzy/DataLV.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Input</t>
   </si>
@@ -51,20 +51,17 @@
     <t>errorAbs</t>
   </si>
   <si>
-    <t>500Intput</t>
+    <t>SciLab</t>
   </si>
   <si>
-    <t>500out</t>
-  </si>
-  <si>
-    <t>SciLab</t>
+    <t>MATLAB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +69,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -89,16 +143,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="40% - Énfasis1" xfId="5" builtinId="31"/>
+    <cellStyle name="40% - Énfasis6" xfId="6" builtinId="51"/>
+    <cellStyle name="Cálculo" xfId="3" builtinId="22"/>
+    <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="4" builtinId="10"/>
+    <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,65 +503,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F27" sqref="E3:F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="L1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3">
@@ -449,29 +594,28 @@
       <c r="F3">
         <v>-100</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>-1.3E-6</v>
       </c>
       <c r="I3" s="1">
         <f>ABS(H3-B3)</f>
         <v>1.3E-6</v>
       </c>
-      <c r="J3" s="1">
-        <f>ABS(I3*100/H3)</f>
-        <v>100.00000000000001</v>
-      </c>
-      <c r="L3">
-        <v>-10</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <f>ABS(L3-B3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C4">
@@ -486,7 +630,7 @@
       <c r="F4">
         <v>-100</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>4.1993500000000003E-2</v>
       </c>
       <c r="I4" s="1">
@@ -497,18 +641,23 @@
         <f t="shared" ref="J4:J23" si="1">ABS(I4*100/H4)</f>
         <v>1.5478585971637423E-2</v>
       </c>
-      <c r="L4">
-        <v>-9</v>
-      </c>
-      <c r="M4">
+      <c r="L4" s="1">
         <v>4.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M23" si="2">ABS(L4-B4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N24" si="3">ABS(M4*100/L4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.13</v>
       </c>
       <c r="C5">
@@ -523,7 +672,7 @@
       <c r="F5">
         <v>-100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>0.12974459999999999</v>
       </c>
       <c r="I5" s="1">
@@ -534,18 +683,23 @@
         <f t="shared" si="1"/>
         <v>0.1968482696004433</v>
       </c>
-      <c r="L5">
-        <v>-8</v>
-      </c>
-      <c r="M5">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="1">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999472E-4</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.23130300693908612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.27700000000000002</v>
       </c>
       <c r="C6">
@@ -560,7 +714,7 @@
       <c r="F6">
         <v>-100</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0.27736509999999998</v>
       </c>
       <c r="I6" s="1">
@@ -571,18 +725,23 @@
         <f t="shared" si="1"/>
         <v>0.13163155710648225</v>
       </c>
-      <c r="L6">
-        <v>-7</v>
-      </c>
-      <c r="M6">
-        <v>0.27700000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <v>0.27739999999999998</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="2"/>
+        <v>3.9999999999995595E-4</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.14419610670510308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.47799999999999998</v>
       </c>
       <c r="C7">
@@ -597,7 +756,7 @@
       <c r="F7">
         <v>-100</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>0.47828599999999999</v>
       </c>
       <c r="I7" s="1">
@@ -608,18 +767,23 @@
         <f t="shared" si="1"/>
         <v>5.9796857946920565E-2</v>
       </c>
-      <c r="L7">
-        <v>-6</v>
-      </c>
-      <c r="M7">
-        <v>0.47799999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="1">
+        <v>0.4783</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0000000000002247E-4</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="3"/>
+        <v>6.2722140915747959E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0.69899999999999995</v>
       </c>
       <c r="C8">
@@ -634,7 +798,7 @@
       <c r="F8">
         <v>-100</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>0.69902529999999996</v>
       </c>
       <c r="I8" s="1">
@@ -645,18 +809,23 @@
         <f t="shared" si="1"/>
         <v>3.619325366335936E-3</v>
       </c>
-      <c r="L8">
-        <v>-5</v>
-      </c>
-      <c r="M8">
+      <c r="L8" s="1">
         <v>0.69899999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-4</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>0.80500000000000005</v>
       </c>
       <c r="C9">
@@ -671,7 +840,7 @@
       <c r="F9">
         <v>-100</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>0.80517609999999995</v>
       </c>
       <c r="I9" s="1">
@@ -682,18 +851,23 @@
         <f t="shared" si="1"/>
         <v>2.1870991948208764E-2</v>
       </c>
-      <c r="L9">
-        <v>-4</v>
-      </c>
-      <c r="M9">
-        <v>0.80500000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="1">
+        <v>0.80520000000000003</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9999999999997797E-4</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="3"/>
+        <v>2.4838549428710627E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-3</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.58299999999999996</v>
       </c>
       <c r="C10">
@@ -708,7 +882,7 @@
       <c r="F10">
         <v>-100</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>0.58326699999999998</v>
       </c>
       <c r="I10" s="1">
@@ -719,18 +893,23 @@
         <f t="shared" si="1"/>
         <v>4.5776634028672498E-2</v>
       </c>
-      <c r="L10">
-        <v>-3</v>
-      </c>
-      <c r="M10">
-        <v>0.58299999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="1">
+        <v>0.58330000000000004</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0000000000007798E-4</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="3"/>
+        <v>5.1431510372034625E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.151</v>
       </c>
       <c r="C11">
@@ -745,7 +924,7 @@
       <c r="F11">
         <v>-100</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0.1515579</v>
       </c>
       <c r="I11" s="1">
@@ -756,18 +935,23 @@
         <f t="shared" si="1"/>
         <v>0.36811014140470411</v>
       </c>
-      <c r="L11">
-        <v>-2</v>
-      </c>
-      <c r="M11">
-        <v>0.151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L11" s="1">
+        <v>0.15160000000000001</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="2"/>
+        <v>6.0000000000001719E-4</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.39577836411610628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>-0.03</v>
       </c>
       <c r="C12">
@@ -782,7 +966,7 @@
       <c r="F12">
         <v>-100</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>-3.0218700000000001E-2</v>
       </c>
       <c r="I12" s="1">
@@ -793,18 +977,23 @@
         <f t="shared" si="1"/>
         <v>0.72372405166338138</v>
       </c>
-      <c r="L12">
-        <v>-1</v>
-      </c>
-      <c r="M12">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" s="1">
+        <v>-3.0200000000000001E-2</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0000000000000226E-4</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.66225165562914656</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13">
@@ -826,22 +1015,21 @@
         <f t="shared" si="0"/>
         <v>5.525E-16</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>3.8780000000000001</v>
       </c>
       <c r="C14">
@@ -856,7 +1044,7 @@
       <c r="F14">
         <v>-100</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>3.8794547000000001</v>
       </c>
       <c r="I14" s="1">
@@ -867,18 +1055,23 @@
         <f t="shared" si="1"/>
         <v>3.749753799161596E-2</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>3.8780000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="1">
+        <v>3.8795000000000002</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5000000000000568E-3</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="3"/>
+        <v>3.8664776388711346E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>1.407</v>
       </c>
       <c r="C15">
@@ -893,7 +1086,7 @@
       <c r="F15">
         <v>-100</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>1.4082948</v>
       </c>
       <c r="I15" s="1">
@@ -904,18 +1097,23 @@
         <f t="shared" si="1"/>
         <v>9.1940977130635523E-2</v>
       </c>
-      <c r="L15">
-        <v>2</v>
-      </c>
-      <c r="M15">
-        <v>1.407</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" s="1">
+        <v>1.4083000000000001</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3000000000000789E-3</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="3"/>
+        <v>9.2309877156861384E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.99299999999999999</v>
       </c>
       <c r="C16">
@@ -930,7 +1128,7 @@
       <c r="F16">
         <v>-100</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>0.99387930000000002</v>
       </c>
       <c r="I16" s="1">
@@ -941,18 +1139,23 @@
         <f t="shared" si="1"/>
         <v>8.8471507556302592E-2</v>
       </c>
-      <c r="L16">
-        <v>3</v>
-      </c>
-      <c r="M16">
-        <v>0.99299999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="1">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>9.000000000000119E-4</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="3"/>
+        <v>9.0552369453668569E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>1.4119999999999999</v>
       </c>
       <c r="C17">
@@ -967,7 +1170,7 @@
       <c r="F17">
         <v>-100</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>1.4124451</v>
       </c>
       <c r="I17" s="1">
@@ -978,18 +1181,23 @@
         <f t="shared" si="1"/>
         <v>3.1512729238119562E-2</v>
       </c>
-      <c r="L17">
-        <v>4</v>
-      </c>
-      <c r="M17">
-        <v>1.4119999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="1">
+        <v>1.4124000000000001</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="2"/>
+        <v>4.0000000000017799E-4</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="3"/>
+        <v>2.832058906826522E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>1.47</v>
       </c>
       <c r="C18">
@@ -1004,7 +1212,7 @@
       <c r="F18">
         <v>-100</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>1.4708175000000001</v>
       </c>
       <c r="I18" s="1">
@@ -1015,18 +1223,23 @@
         <f t="shared" si="1"/>
         <v>5.5581334869903132E-2</v>
       </c>
-      <c r="L18">
-        <v>5</v>
-      </c>
-      <c r="M18">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="1">
+        <v>1.4708000000000001</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="2"/>
+        <v>8.0000000000013394E-4</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="3"/>
+        <v>5.4392167527885088E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>1.17</v>
       </c>
       <c r="C19">
@@ -1041,7 +1254,7 @@
       <c r="F19">
         <v>-100</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>1.1705053000000001</v>
       </c>
       <c r="I19" s="1">
@@ -1052,18 +1265,23 @@
         <f t="shared" si="1"/>
         <v>4.3169390177058814E-2</v>
       </c>
-      <c r="L19">
-        <v>6</v>
-      </c>
-      <c r="M19">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="1">
+        <v>1.1705000000000001</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0000000000016698E-4</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="3"/>
+        <v>4.2716787697579403E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.64600000000000002</v>
       </c>
       <c r="C20">
@@ -1078,7 +1296,7 @@
       <c r="F20">
         <v>-100</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <v>0.64611569999999996</v>
       </c>
       <c r="I20" s="1">
@@ -1089,18 +1307,23 @@
         <f t="shared" si="1"/>
         <v>1.7907009534041791E-2</v>
       </c>
-      <c r="L20">
-        <v>7</v>
-      </c>
-      <c r="M20">
-        <v>0.64600000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <v>0.64610000000000001</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="2"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5477480266210956E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0.44800000000000001</v>
       </c>
       <c r="C21">
@@ -1115,7 +1338,7 @@
       <c r="F21">
         <v>-100</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>0.44823730000000001</v>
       </c>
       <c r="I21" s="1">
@@ -1126,18 +1349,23 @@
         <f t="shared" si="1"/>
         <v>5.2940707968746878E-2</v>
       </c>
-      <c r="L21">
-        <v>8</v>
-      </c>
-      <c r="M21">
-        <v>0.44800000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="1">
+        <v>0.44819999999999999</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9999999999997797E-4</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4622936189196334E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.247</v>
       </c>
       <c r="C22">
@@ -1152,7 +1380,7 @@
       <c r="F22">
         <v>-50</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>0.24785679999999999</v>
       </c>
       <c r="I22" s="1">
@@ -1163,18 +1391,23 @@
         <f t="shared" si="1"/>
         <v>0.3456834752970227</v>
       </c>
-      <c r="L22">
-        <v>9</v>
-      </c>
-      <c r="M22">
-        <v>0.247</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="1">
+        <v>0.24790000000000001</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="2"/>
+        <v>9.000000000000119E-4</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="3"/>
+        <v>0.36304961678096487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.19</v>
       </c>
       <c r="C23">
@@ -1189,25 +1422,30 @@
       <c r="F23">
         <v>-100</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <v>0.19081290000000001</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="2">
         <f t="shared" si="0"/>
         <v>8.1290000000000529E-4</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="2">
         <f t="shared" si="1"/>
         <v>0.42601941482992256</v>
       </c>
-      <c r="L23">
-        <v>10</v>
-      </c>
-      <c r="M23">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="2">
+        <v>0.1908</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9999999999999516E-4</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.41928721174003941</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>1</v>
       </c>
@@ -1220,8 +1458,17 @@
       <c r="F24">
         <v>-100</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+      <c r="J24" s="3">
+        <f>SUM(J4:J23)/25</f>
+        <v>0.11030321998520626</v>
+      </c>
+      <c r="N24" s="3">
+        <f>SUM(N4:N23)/25</f>
+        <v>0.11047660585501271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>1</v>
       </c>
@@ -1234,8 +1481,9 @@
       <c r="F25">
         <v>-100</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
@@ -1249,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>1</v>
       </c>

</xml_diff>